<commit_message>
Rodando com Combinações de Estratégias
</commit_message>
<xml_diff>
--- a/models/difusion-model/params.xlsx
+++ b/models/difusion-model/params.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\ms-rdm-dissertation\current_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\ms-rdm-dissertation\models\difusion-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3" xr2:uid="{8C8B848D-7755-48BA-85DF-1CF1830EFE49}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{8C8B848D-7755-48BA-85DF-1CF1830EFE49}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
-    <sheet name="configs" sheetId="2" r:id="rId2"/>
-    <sheet name="VariableNames" sheetId="3" r:id="rId3"/>
-    <sheet name="levers" sheetId="4" r:id="rId4"/>
+    <sheet name="levers" sheetId="4" r:id="rId2"/>
+    <sheet name="configs" sheetId="2" r:id="rId3"/>
+    <sheet name="VariableNames" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>Variavel</t>
   </si>
@@ -167,13 +167,25 @@
     <t>Anos</t>
   </si>
   <si>
-    <t>Parametro1</t>
-  </si>
-  <si>
-    <t>Parametro2</t>
-  </si>
-  <si>
     <t>Lever</t>
+  </si>
+  <si>
+    <t>aAdvertisingON</t>
+  </si>
+  <si>
+    <t>aAdvertisingIntensity</t>
+  </si>
+  <si>
+    <t>LeverCode</t>
+  </si>
+  <si>
+    <t>NADV</t>
+  </si>
+  <si>
+    <t>ads</t>
+  </si>
+  <si>
+    <t>adsa</t>
   </si>
 </sst>
 </file>
@@ -537,7 +549,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3AF1C2-6E06-403B-B596-52A55D7EBB3C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -632,6 +646,20 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
     </row>
@@ -642,6 +670,116 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15055839-DAEF-45EB-940F-B4DD495D311F}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>"ADV-"&amp;D2</f>
+        <v>ADV-1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f>"ADV-"&amp;D3</f>
+        <v>ADV-2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f>"ADV-"&amp;D4</f>
+        <v>ADV-3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f>"ADV-"&amp;D5</f>
+        <v>ADV-4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5C43C2-1FAB-479F-820C-4D2F1DEEC0BC}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -677,7 +815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC23235-B0D4-47B4-91CF-02E948D7C177}">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -834,77 +972,4 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15055839-DAEF-45EB-940F-B4DD495D311F}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Alterações em Análise - Comparando as Estratégias Diferentes
</commit_message>
<xml_diff>
--- a/models/difusion-model/params.xlsx
+++ b/models/difusion-model/params.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{8C8B848D-7755-48BA-85DF-1CF1830EFE49}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{8C8B848D-7755-48BA-85DF-1CF1830EFE49}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -549,9 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3AF1C2-6E06-403B-B596-52A55D7EBB3C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -673,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15055839-DAEF-45EB-940F-B4DD495D311F}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Análise funcionando com filtro por Estratégia
</commit_message>
<xml_diff>
--- a/models/difusion-model/params.xlsx
+++ b/models/difusion-model/params.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>Variavel</t>
   </si>
@@ -180,12 +180,6 @@
   </si>
   <si>
     <t>NADV</t>
-  </si>
-  <si>
-    <t>ads</t>
-  </si>
-  <si>
-    <t>adsa</t>
   </si>
 </sst>
 </file>
@@ -547,9 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3AF1C2-6E06-403B-B596-52A55D7EBB3C}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -645,21 +641,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
+      <c r="B6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -672,7 +654,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Importando Modelo Original para realizar a Análise RDM completa no modelo de Bass
</commit_message>
<xml_diff>
--- a/models/difusion-model/params.xlsx
+++ b/models/difusion-model/params.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Variavel</t>
   </si>
@@ -177,16 +177,28 @@
   </si>
   <si>
     <t>LeverCode</t>
-  </si>
-  <si>
-    <t>NADV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,10 +235,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,104 +558,106 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="62" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="62" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2">
-        <v>0.01</v>
-      </c>
-      <c r="D2">
-        <v>0.1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
+        <v>50</v>
+      </c>
+      <c r="D3" s="3">
+        <v>200</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
-        <v>0.01</v>
-      </c>
-      <c r="D4">
-        <v>0.1</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>1000000</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>1000000</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
+      <c r="B6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -651,7 +667,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15055839-DAEF-45EB-940F-B4DD495D311F}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -685,13 +701,13 @@
       </c>
       <c r="B2" t="str">
         <f>"ADV-"&amp;D2</f>
-        <v>ADV-1</v>
+        <v>ADV-2</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -700,56 +716,12 @@
       </c>
       <c r="B3" t="str">
         <f>"ADV-"&amp;D3</f>
-        <v>ADV-2</v>
+        <v>ADV-0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="str">
-        <f>"ADV-"&amp;D4</f>
-        <v>ADV-3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="str">
-        <f>"ADV-"&amp;D5</f>
-        <v>ADV-4</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rodando a etapa de escolha das melhores estratégias pelo regret (quartil)
</commit_message>
<xml_diff>
--- a/models/difusion-model/params.xlsx
+++ b/models/difusion-model/params.xlsx
@@ -558,7 +558,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,10 +667,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15055839-DAEF-45EB-940F-B4DD495D311F}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,14 +700,14 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <f>"ADV-"&amp;D2</f>
-        <v>ADV-2</v>
+        <f t="shared" ref="B2:B9" si="0">"ADV-"&amp;D2</f>
+        <v>ADV-1</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -715,13 +715,109 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <f>"ADV-"&amp;D3</f>
+        <f t="shared" si="0"/>
+        <v>ADV-1,5</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D8" si="1">D2+0.5</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>ADV-2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>ADV-2,5</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>ADV-3</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>ADV-3,5</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>ADV-4</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
         <v>ADV-0</v>
       </c>
-      <c r="C3">
+      <c r="C9">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="D9">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Análises com Regret por Estratégia (Gráfico Whisker)
</commit_message>
<xml_diff>
--- a/models/difusion-model/params.xlsx
+++ b/models/difusion-model/params.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{8C8B848D-7755-48BA-85DF-1CF1830EFE49}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{8C8B848D-7755-48BA-85DF-1CF1830EFE49}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>Variavel</t>
   </si>
@@ -177,6 +177,24 @@
   </si>
   <si>
     <t>LeverCode</t>
+  </si>
+  <si>
+    <t>aAverageTicket</t>
+  </si>
+  <si>
+    <t>TicketMedio</t>
+  </si>
+  <si>
+    <t>{Reais / pessoa / ano}</t>
+  </si>
+  <si>
+    <t>aAdvertisingCost</t>
+  </si>
+  <si>
+    <t>Custo da Propaganda</t>
+  </si>
+  <si>
+    <t>{Reais / Nível de Intensidade}</t>
   </si>
 </sst>
 </file>
@@ -207,7 +225,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -235,10 +252,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -555,109 +571,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3AF1C2-6E06-403B-B596-52A55D7EBB3C}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="3"/>
-    <col min="5" max="5" width="62" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="62" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
         <v>50</v>
       </c>
-      <c r="D3" s="3">
-        <v>200</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>0</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0.03</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>1000000</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>1000000</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
+      <c r="A6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="D6" s="2">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>100000</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -667,157 +714,350 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15055839-DAEF-45EB-940F-B4DD495D311F}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="str">
-        <f t="shared" ref="B2:B9" si="0">"ADV-"&amp;D2</f>
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="str">
+        <f t="shared" ref="B2:B21" si="0">"ADV-"&amp;D2</f>
         <v>ADV-1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ADV-1,5</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D8" si="1">D2+0.5</f>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D20" si="1">D2+0.5</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B4" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ADV-2</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ADV-2,5</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ADV-3</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ADV-3,5</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
         <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ADV-4</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B9" s="3" t="str">
+        <f t="shared" ref="B9:B20" si="2">"ADV-"&amp;D9</f>
+        <v>ADV-4,5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ADV-5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ADV-5,5</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ADV-6</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ADV-6,5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ADV-7</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ADV-7,5</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ADV-8</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ADV-8,5</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ADV-9</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ADV-9,5</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="1"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>ADV-10</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ADV-0</v>
       </c>
-      <c r="C9">
+      <c r="C21" s="3">
         <v>0</v>
       </c>
-      <c r="D9">
+      <c r="D21" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Generalização do RDM e escolha da estratégia finalizada!
</commit_message>
<xml_diff>
--- a/models/difusion-model/params.xlsx
+++ b/models/difusion-model/params.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{8C8B848D-7755-48BA-85DF-1CF1830EFE49}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{8C8B848D-7755-48BA-85DF-1CF1830EFE49}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3AF1C2-6E06-403B-B596-52A55D7EBB3C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,10 +629,10 @@
         <v>14</v>
       </c>
       <c r="C3" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>9</v>
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15055839-DAEF-45EB-940F-B4DD495D311F}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implementando gráfico em matriz. depois substituir com a biblioteca ggaly
</commit_message>
<xml_diff>
--- a/models/difusion-model/params.xlsx
+++ b/models/difusion-model/params.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -53,9 +53,6 @@
     <t>Unidade</t>
   </si>
   <si>
-    <t>{1/year}</t>
-  </si>
-  <si>
     <t>{people per person/year, which simplifies dimensionally to 1/year}</t>
   </si>
   <si>
@@ -195,6 +192,9 @@
   </si>
   <si>
     <t>{Reais / Nível de Intensidade}</t>
+  </si>
+  <si>
+    <t>{1/ano}</t>
   </si>
 </sst>
 </file>
@@ -252,11 +252,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,7 +574,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3AF1C2-6E06-403B-B596-52A55D7EBB3C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -590,7 +593,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -607,16 +610,16 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D2" s="3">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -624,16 +627,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3">
-        <v>100</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>80</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -641,16 +644,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D4" s="3">
         <v>0.03</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -658,7 +661,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3">
         <v>1000000</v>
@@ -667,41 +670,42 @@
         <v>1000000</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="C6" s="3">
-        <v>0.01</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3">
         <v>10</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="C7" s="3">
-        <v>1</v>
+        <f>D7/3</f>
+        <v>33333.333333333336</v>
       </c>
       <c r="D7" s="3">
         <v>100000</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -715,7 +719,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D18"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,16 +733,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1070,20 +1074,20 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1121,140 +1125,140 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrigindo erro no gráfico de estratégias vs incertezas
</commit_message>
<xml_diff>
--- a/models/difusion-model/params.xlsx
+++ b/models/difusion-model/params.xlsx
@@ -574,9 +574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3AF1C2-6E06-403B-B596-52A55D7EBB3C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -718,9 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15055839-DAEF-45EB-940F-B4DD495D311F}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -750,14 +746,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="str">
-        <f t="shared" ref="B2:B21" si="0">"ADV-"&amp;D2</f>
-        <v>ADV-1</v>
+        <f t="shared" ref="B2" si="0">"ADV-"&amp;D2</f>
+        <v>ADV-0</v>
       </c>
       <c r="C2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -765,15 +761,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ADV-1,5</v>
+        <f t="shared" ref="B3:B9" si="1">"ADV-"&amp;D3</f>
+        <v>ADV-1</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D20" si="1">D2+0.5</f>
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -781,15 +776,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ADV-2</v>
+        <f t="shared" si="1"/>
+        <v>ADV-1,5</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f t="shared" ref="D4:D21" si="2">D3+0.5</f>
+        <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -797,15 +792,15 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ADV-2,5</v>
+        <f t="shared" si="1"/>
+        <v>ADV-2</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -813,15 +808,15 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ADV-3</v>
+        <f t="shared" si="1"/>
+        <v>ADV-2,5</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>2.5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -829,15 +824,15 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ADV-3,5</v>
+        <f t="shared" si="1"/>
+        <v>ADV-3</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="1"/>
-        <v>3.5</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -845,15 +840,15 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ADV-4</v>
+        <f t="shared" si="1"/>
+        <v>ADV-3,5</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>3.5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -861,15 +856,15 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="str">
-        <f t="shared" ref="B9:B20" si="2">"ADV-"&amp;D9</f>
-        <v>ADV-4,5</v>
+        <f t="shared" si="1"/>
+        <v>ADV-4</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="1"/>
-        <v>4.5</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -877,15 +872,15 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>ADV-5</v>
+        <f t="shared" ref="B10:B21" si="3">"ADV-"&amp;D10</f>
+        <v>ADV-4,5</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>4.5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -893,15 +888,15 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>ADV-5,5</v>
+        <f t="shared" si="3"/>
+        <v>ADV-5</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="1"/>
-        <v>5.5</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -909,15 +904,15 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>ADV-6</v>
+        <f t="shared" si="3"/>
+        <v>ADV-5,5</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>5.5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -925,15 +920,15 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>ADV-6,5</v>
+        <f t="shared" si="3"/>
+        <v>ADV-6</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="1"/>
-        <v>6.5</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -941,15 +936,15 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>ADV-7</v>
+        <f t="shared" si="3"/>
+        <v>ADV-6,5</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f t="shared" si="2"/>
+        <v>6.5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -957,15 +952,15 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>ADV-7,5</v>
+        <f t="shared" si="3"/>
+        <v>ADV-7</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" si="1"/>
-        <v>7.5</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -973,15 +968,15 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>ADV-8</v>
+        <f t="shared" si="3"/>
+        <v>ADV-7,5</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>7.5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -989,15 +984,15 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>ADV-8,5</v>
+        <f t="shared" si="3"/>
+        <v>ADV-8</v>
       </c>
       <c r="C17" s="2">
         <v>1</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="1"/>
-        <v>8.5</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1005,15 +1000,15 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>ADV-9</v>
+        <f t="shared" si="3"/>
+        <v>ADV-8,5</v>
       </c>
       <c r="C18" s="2">
         <v>1</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f t="shared" si="2"/>
+        <v>8.5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1021,15 +1016,15 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>ADV-9,5</v>
+        <f t="shared" si="3"/>
+        <v>ADV-9</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" si="1"/>
-        <v>9.5</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1037,15 +1032,15 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>ADV-10</v>
+        <f t="shared" si="3"/>
+        <v>ADV-9,5</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>9.5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1053,14 +1048,15 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ADV-0</v>
+        <f t="shared" si="3"/>
+        <v>ADV-10</v>
       </c>
       <c r="C21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>